<commit_message>
update migration and seed
</commit_message>
<xml_diff>
--- a/cheklist_kebersihan.xlsx
+++ b/cheklist_kebersihan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp2\Documents\Bionic\bionic\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F7499C-EABB-41C8-B4D1-C7D946745333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D029ACE-1D93-446D-8900-275A311F5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3270" yWindow="1245" windowWidth="21015" windowHeight="11295" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1607,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(OR(B2="sabun_cuci_tangan",B2="tisu",B2="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F2:F33" si="0">IF(OR(B2="sabun_cuci_tangan",B2="tisu",B2="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(OR(B3="sabun_cuci_tangan",B3="tisu",B3="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(OR(B4="sabun_cuci_tangan",B4="tisu",B4="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(OR(B5="sabun_cuci_tangan",B5="tisu",B5="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(OR(B6="sabun_cuci_tangan",B6="tisu",B6="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1722,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(OR(B7="sabun_cuci_tangan",B7="tisu",B7="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(OR(B8="sabun_cuci_tangan",B8="tisu",B8="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(OR(B9="sabun_cuci_tangan",B9="tisu",B9="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(OR(B10="sabun_cuci_tangan",B10="tisu",B10="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(OR(B11="sabun_cuci_tangan",B11="tisu",B11="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(OR(B12="sabun_cuci_tangan",B12="tisu",B12="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1860,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(OR(B13="sabun_cuci_tangan",B13="tisu",B13="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(OR(B14="sabun_cuci_tangan",B14="tisu",B14="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(OR(B15="sabun_cuci_tangan",B15="tisu",B15="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(OR(B16="sabun_cuci_tangan",B16="tisu",B16="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1952,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(OR(B17="sabun_cuci_tangan",B17="tisu",B17="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
         <v>2</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(OR(B18="sabun_cuci_tangan",B18="tisu",B18="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -1998,7 +1998,7 @@
         <v>2</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(OR(B19="sabun_cuci_tangan",B19="tisu",B19="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(OR(B20="sabun_cuci_tangan",B20="tisu",B20="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
         <v>3</v>
       </c>
       <c r="F21" t="str">
-        <f>IF(OR(B21="sabun_cuci_tangan",B21="tisu",B21="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
         <v>3</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(OR(B22="sabun_cuci_tangan",B22="tisu",B22="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
         <v>3</v>
       </c>
       <c r="F23" t="str">
-        <f>IF(OR(B23="sabun_cuci_tangan",B23="tisu",B23="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(OR(B24="sabun_cuci_tangan",B24="tisu",B24="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="F25" t="str">
-        <f>IF(OR(B25="sabun_cuci_tangan",B25="tisu",B25="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
         <v>3</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(OR(B26="sabun_cuci_tangan",B26="tisu",B26="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2182,7 +2182,7 @@
         <v>3</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(OR(B27="sabun_cuci_tangan",B27="tisu",B27="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
         <v>4</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(OR(B28="sabun_cuci_tangan",B28="tisu",B28="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2228,7 +2228,7 @@
         <v>4</v>
       </c>
       <c r="F29" t="str">
-        <f>IF(OR(B29="sabun_cuci_tangan",B29="tisu",B29="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
         <v>4</v>
       </c>
       <c r="F30" t="str">
-        <f>IF(OR(B30="sabun_cuci_tangan",B30="tisu",B30="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
         <v>4</v>
       </c>
       <c r="F31" t="str">
-        <f>IF(OR(B31="sabun_cuci_tangan",B31="tisu",B31="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="F32" t="str">
-        <f>IF(OR(B32="sabun_cuci_tangan",B32="tisu",B32="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
         <v>4</v>
       </c>
       <c r="F33" t="str">
-        <f>IF(OR(B33="sabun_cuci_tangan",B33="tisu",B33="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
         <v>4</v>
       </c>
       <c r="F34" t="str">
-        <f>IF(OR(B34="sabun_cuci_tangan",B34="tisu",B34="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F34:F65" si="1">IF(OR(B34="sabun_cuci_tangan",B34="tisu",B34="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
         <v>4</v>
       </c>
       <c r="F35" t="str">
-        <f>IF(OR(B35="sabun_cuci_tangan",B35="tisu",B35="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
         <v>5</v>
       </c>
       <c r="F36" t="str">
-        <f>IF(OR(B36="sabun_cuci_tangan",B36="tisu",B36="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2412,7 +2412,7 @@
         <v>5</v>
       </c>
       <c r="F37" t="str">
-        <f>IF(OR(B37="sabun_cuci_tangan",B37="tisu",B37="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="F38" t="str">
-        <f>IF(OR(B38="sabun_cuci_tangan",B38="tisu",B38="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
         <v>5</v>
       </c>
       <c r="F39" t="str">
-        <f>IF(OR(B39="sabun_cuci_tangan",B39="tisu",B39="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
         <v>5</v>
       </c>
       <c r="F40" t="str">
-        <f>IF(OR(B40="sabun_cuci_tangan",B40="tisu",B40="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2504,7 +2504,7 @@
         <v>5</v>
       </c>
       <c r="F41" t="str">
-        <f>IF(OR(B41="sabun_cuci_tangan",B41="tisu",B41="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2527,7 +2527,7 @@
         <v>5</v>
       </c>
       <c r="F42" t="str">
-        <f>IF(OR(B42="sabun_cuci_tangan",B42="tisu",B42="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2550,7 +2550,7 @@
         <v>5</v>
       </c>
       <c r="F43" t="str">
-        <f>IF(OR(B43="sabun_cuci_tangan",B43="tisu",B43="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2573,7 +2573,7 @@
         <v>5</v>
       </c>
       <c r="F44" t="str">
-        <f>IF(OR(B44="sabun_cuci_tangan",B44="tisu",B44="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2596,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="F45" t="str">
-        <f>IF(OR(B45="sabun_cuci_tangan",B45="tisu",B45="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>refill</v>
       </c>
     </row>
@@ -2619,7 +2619,7 @@
         <v>6</v>
       </c>
       <c r="F46" t="str">
-        <f>IF(OR(B46="sabun_cuci_tangan",B46="tisu",B46="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2642,7 +2642,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="str">
-        <f>IF(OR(B47="sabun_cuci_tangan",B47="tisu",B47="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="str">
-        <f>IF(OR(B48="sabun_cuci_tangan",B48="tisu",B48="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2688,7 +2688,7 @@
         <v>6</v>
       </c>
       <c r="F49" t="str">
-        <f>IF(OR(B49="sabun_cuci_tangan",B49="tisu",B49="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
         <v>6</v>
       </c>
       <c r="F50" t="str">
-        <f>IF(OR(B50="sabun_cuci_tangan",B50="tisu",B50="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2734,7 +2734,7 @@
         <v>6</v>
       </c>
       <c r="F51" t="str">
-        <f>IF(OR(B51="sabun_cuci_tangan",B51="tisu",B51="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>refill</v>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
         <v>6</v>
       </c>
       <c r="F52" t="str">
-        <f>IF(OR(B52="sabun_cuci_tangan",B52="tisu",B52="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2780,7 +2780,7 @@
         <v>6</v>
       </c>
       <c r="F53" t="str">
-        <f>IF(OR(B53="sabun_cuci_tangan",B53="tisu",B53="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
       <c r="F54" t="str">
-        <f>IF(OR(B54="sabun_cuci_tangan",B54="tisu",B54="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>refill</v>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
         <v>6</v>
       </c>
       <c r="F55" t="str">
-        <f>IF(OR(B55="sabun_cuci_tangan",B55="tisu",B55="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>refill</v>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
         <v>7</v>
       </c>
       <c r="F56" t="str">
-        <f>IF(OR(B56="sabun_cuci_tangan",B56="tisu",B56="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2872,7 +2872,7 @@
         <v>7</v>
       </c>
       <c r="F57" t="str">
-        <f>IF(OR(B57="sabun_cuci_tangan",B57="tisu",B57="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2895,7 +2895,7 @@
         <v>7</v>
       </c>
       <c r="F58" t="str">
-        <f>IF(OR(B58="sabun_cuci_tangan",B58="tisu",B58="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2918,7 +2918,7 @@
         <v>7</v>
       </c>
       <c r="F59" t="str">
-        <f>IF(OR(B59="sabun_cuci_tangan",B59="tisu",B59="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2941,7 +2941,7 @@
         <v>7</v>
       </c>
       <c r="F60" t="str">
-        <f>IF(OR(B60="sabun_cuci_tangan",B60="tisu",B60="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2964,7 +2964,7 @@
         <v>8</v>
       </c>
       <c r="F61" t="str">
-        <f>IF(OR(B61="sabun_cuci_tangan",B61="tisu",B61="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
         <v>8</v>
       </c>
       <c r="F62" t="str">
-        <f>IF(OR(B62="sabun_cuci_tangan",B62="tisu",B62="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3010,7 +3010,7 @@
         <v>8</v>
       </c>
       <c r="F63" t="str">
-        <f>IF(OR(B63="sabun_cuci_tangan",B63="tisu",B63="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3033,7 +3033,7 @@
         <v>8</v>
       </c>
       <c r="F64" t="str">
-        <f>IF(OR(B64="sabun_cuci_tangan",B64="tisu",B64="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3056,7 +3056,7 @@
         <v>8</v>
       </c>
       <c r="F65" t="str">
-        <f>IF(OR(B65="sabun_cuci_tangan",B65="tisu",B65="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3079,7 +3079,7 @@
         <v>8</v>
       </c>
       <c r="F66" t="str">
-        <f>IF(OR(B66="sabun_cuci_tangan",B66="tisu",B66="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F66:F97" si="2">IF(OR(B66="sabun_cuci_tangan",B66="tisu",B66="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
         <v>8</v>
       </c>
       <c r="F67" t="str">
-        <f>IF(OR(B67="sabun_cuci_tangan",B67="tisu",B67="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3125,7 +3125,7 @@
         <v>8</v>
       </c>
       <c r="F68" t="str">
-        <f>IF(OR(B68="sabun_cuci_tangan",B68="tisu",B68="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3148,7 +3148,7 @@
         <v>9</v>
       </c>
       <c r="F69" t="str">
-        <f>IF(OR(B69="sabun_cuci_tangan",B69="tisu",B69="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3171,7 +3171,7 @@
         <v>9</v>
       </c>
       <c r="F70" t="str">
-        <f>IF(OR(B70="sabun_cuci_tangan",B70="tisu",B70="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
         <v>9</v>
       </c>
       <c r="F71" t="str">
-        <f>IF(OR(B71="sabun_cuci_tangan",B71="tisu",B71="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
         <v>9</v>
       </c>
       <c r="F72" t="str">
-        <f>IF(OR(B72="sabun_cuci_tangan",B72="tisu",B72="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3240,7 +3240,7 @@
         <v>9</v>
       </c>
       <c r="F73" t="str">
-        <f>IF(OR(B73="sabun_cuci_tangan",B73="tisu",B73="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3263,7 +3263,7 @@
         <v>9</v>
       </c>
       <c r="F74" t="str">
-        <f>IF(OR(B74="sabun_cuci_tangan",B74="tisu",B74="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="F75" t="str">
-        <f>IF(OR(B75="sabun_cuci_tangan",B75="tisu",B75="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3309,7 +3309,7 @@
         <v>9</v>
       </c>
       <c r="F76" t="str">
-        <f>IF(OR(B76="sabun_cuci_tangan",B76="tisu",B76="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3332,7 +3332,7 @@
         <v>9</v>
       </c>
       <c r="F77" t="str">
-        <f>IF(OR(B77="sabun_cuci_tangan",B77="tisu",B77="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
         <v>9</v>
       </c>
       <c r="F78" t="str">
-        <f>IF(OR(B78="sabun_cuci_tangan",B78="tisu",B78="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3378,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="F79" t="str">
-        <f>IF(OR(B79="sabun_cuci_tangan",B79="tisu",B79="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3401,7 +3401,7 @@
         <v>10</v>
       </c>
       <c r="F80" t="str">
-        <f>IF(OR(B80="sabun_cuci_tangan",B80="tisu",B80="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3424,7 +3424,7 @@
         <v>10</v>
       </c>
       <c r="F81" t="str">
-        <f>IF(OR(B81="sabun_cuci_tangan",B81="tisu",B81="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3447,7 +3447,7 @@
         <v>10</v>
       </c>
       <c r="F82" t="str">
-        <f>IF(OR(B82="sabun_cuci_tangan",B82="tisu",B82="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
         <v>10</v>
       </c>
       <c r="F83" t="str">
-        <f>IF(OR(B83="sabun_cuci_tangan",B83="tisu",B83="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3493,7 +3493,7 @@
         <v>10</v>
       </c>
       <c r="F84" t="str">
-        <f>IF(OR(B84="sabun_cuci_tangan",B84="tisu",B84="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>refill</v>
       </c>
     </row>
@@ -3516,7 +3516,7 @@
         <v>10</v>
       </c>
       <c r="F85" t="str">
-        <f>IF(OR(B85="sabun_cuci_tangan",B85="tisu",B85="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3539,7 +3539,7 @@
         <v>10</v>
       </c>
       <c r="F86" t="str">
-        <f>IF(OR(B86="sabun_cuci_tangan",B86="tisu",B86="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3562,7 +3562,7 @@
         <v>10</v>
       </c>
       <c r="F87" t="str">
-        <f>IF(OR(B87="sabun_cuci_tangan",B87="tisu",B87="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3585,7 +3585,7 @@
         <v>11</v>
       </c>
       <c r="F88" t="str">
-        <f>IF(OR(B88="sabun_cuci_tangan",B88="tisu",B88="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3608,7 +3608,7 @@
         <v>11</v>
       </c>
       <c r="F89" t="str">
-        <f>IF(OR(B89="sabun_cuci_tangan",B89="tisu",B89="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3631,7 +3631,7 @@
         <v>11</v>
       </c>
       <c r="F90" t="str">
-        <f>IF(OR(B90="sabun_cuci_tangan",B90="tisu",B90="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3654,7 +3654,7 @@
         <v>11</v>
       </c>
       <c r="F91" t="str">
-        <f>IF(OR(B91="sabun_cuci_tangan",B91="tisu",B91="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
         <v>11</v>
       </c>
       <c r="F92" t="str">
-        <f>IF(OR(B92="sabun_cuci_tangan",B92="tisu",B92="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3700,7 +3700,7 @@
         <v>11</v>
       </c>
       <c r="F93" t="str">
-        <f>IF(OR(B93="sabun_cuci_tangan",B93="tisu",B93="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>refill</v>
       </c>
     </row>
@@ -3723,7 +3723,7 @@
         <v>11</v>
       </c>
       <c r="F94" t="str">
-        <f>IF(OR(B94="sabun_cuci_tangan",B94="tisu",B94="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3746,7 +3746,7 @@
         <v>11</v>
       </c>
       <c r="F95" t="str">
-        <f>IF(OR(B95="sabun_cuci_tangan",B95="tisu",B95="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
         <v>11</v>
       </c>
       <c r="F96" t="str">
-        <f>IF(OR(B96="sabun_cuci_tangan",B96="tisu",B96="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>refill</v>
       </c>
     </row>
@@ -3792,7 +3792,7 @@
         <v>11</v>
       </c>
       <c r="F97" t="str">
-        <f>IF(OR(B97="sabun_cuci_tangan",B97="tisu",B97="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>refill</v>
       </c>
     </row>
@@ -3815,7 +3815,7 @@
         <v>11</v>
       </c>
       <c r="F98" t="str">
-        <f>IF(OR(B98="sabun_cuci_tangan",B98="tisu",B98="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F98:F129" si="3">IF(OR(B98="sabun_cuci_tangan",B98="tisu",B98="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -3838,7 +3838,7 @@
         <v>12</v>
       </c>
       <c r="F99" t="str">
-        <f>IF(OR(B99="sabun_cuci_tangan",B99="tisu",B99="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
         <v>12</v>
       </c>
       <c r="F100" t="str">
-        <f>IF(OR(B100="sabun_cuci_tangan",B100="tisu",B100="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
         <v>12</v>
       </c>
       <c r="F101" t="str">
-        <f>IF(OR(B101="sabun_cuci_tangan",B101="tisu",B101="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3907,7 +3907,7 @@
         <v>12</v>
       </c>
       <c r="F102" t="str">
-        <f>IF(OR(B102="sabun_cuci_tangan",B102="tisu",B102="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3930,7 +3930,7 @@
         <v>12</v>
       </c>
       <c r="F103" t="str">
-        <f>IF(OR(B103="sabun_cuci_tangan",B103="tisu",B103="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3953,7 +3953,7 @@
         <v>12</v>
       </c>
       <c r="F104" t="str">
-        <f>IF(OR(B104="sabun_cuci_tangan",B104="tisu",B104="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3976,7 +3976,7 @@
         <v>13</v>
       </c>
       <c r="F105" t="str">
-        <f>IF(OR(B105="sabun_cuci_tangan",B105="tisu",B105="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -3999,7 +3999,7 @@
         <v>13</v>
       </c>
       <c r="F106" t="str">
-        <f>IF(OR(B106="sabun_cuci_tangan",B106="tisu",B106="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4022,7 +4022,7 @@
         <v>13</v>
       </c>
       <c r="F107" t="str">
-        <f>IF(OR(B107="sabun_cuci_tangan",B107="tisu",B107="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4045,7 +4045,7 @@
         <v>13</v>
       </c>
       <c r="F108" t="str">
-        <f>IF(OR(B108="sabun_cuci_tangan",B108="tisu",B108="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4068,7 +4068,7 @@
         <v>13</v>
       </c>
       <c r="F109" t="str">
-        <f>IF(OR(B109="sabun_cuci_tangan",B109="tisu",B109="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>refill</v>
       </c>
     </row>
@@ -4091,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="F110" t="str">
-        <f>IF(OR(B110="sabun_cuci_tangan",B110="tisu",B110="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4114,7 +4114,7 @@
         <v>13</v>
       </c>
       <c r="F111" t="str">
-        <f>IF(OR(B111="sabun_cuci_tangan",B111="tisu",B111="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
         <v>13</v>
       </c>
       <c r="F112" t="str">
-        <f>IF(OR(B112="sabun_cuci_tangan",B112="tisu",B112="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4160,7 +4160,7 @@
         <v>14</v>
       </c>
       <c r="F113" t="str">
-        <f>IF(OR(B113="sabun_cuci_tangan",B113="tisu",B113="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4183,7 +4183,7 @@
         <v>14</v>
       </c>
       <c r="F114" t="str">
-        <f>IF(OR(B114="sabun_cuci_tangan",B114="tisu",B114="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
         <v>14</v>
       </c>
       <c r="F115" t="str">
-        <f>IF(OR(B115="sabun_cuci_tangan",B115="tisu",B115="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
         <v>14</v>
       </c>
       <c r="F116" t="str">
-        <f>IF(OR(B116="sabun_cuci_tangan",B116="tisu",B116="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4252,7 +4252,7 @@
         <v>14</v>
       </c>
       <c r="F117" t="str">
-        <f>IF(OR(B117="sabun_cuci_tangan",B117="tisu",B117="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
         <v>14</v>
       </c>
       <c r="F118" t="str">
-        <f>IF(OR(B118="sabun_cuci_tangan",B118="tisu",B118="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4298,7 +4298,7 @@
         <v>14</v>
       </c>
       <c r="F119" t="str">
-        <f>IF(OR(B119="sabun_cuci_tangan",B119="tisu",B119="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4321,7 +4321,7 @@
         <v>14</v>
       </c>
       <c r="F120" t="str">
-        <f>IF(OR(B120="sabun_cuci_tangan",B120="tisu",B120="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
         <v>15</v>
       </c>
       <c r="F121" t="str">
-        <f>IF(OR(B121="sabun_cuci_tangan",B121="tisu",B121="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4367,7 +4367,7 @@
         <v>15</v>
       </c>
       <c r="F122" t="str">
-        <f>IF(OR(B122="sabun_cuci_tangan",B122="tisu",B122="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4390,7 +4390,7 @@
         <v>15</v>
       </c>
       <c r="F123" t="str">
-        <f>IF(OR(B123="sabun_cuci_tangan",B123="tisu",B123="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4413,7 +4413,7 @@
         <v>15</v>
       </c>
       <c r="F124" t="str">
-        <f>IF(OR(B124="sabun_cuci_tangan",B124="tisu",B124="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4436,7 +4436,7 @@
         <v>15</v>
       </c>
       <c r="F125" t="str">
-        <f>IF(OR(B125="sabun_cuci_tangan",B125="tisu",B125="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4459,7 +4459,7 @@
         <v>15</v>
       </c>
       <c r="F126" t="str">
-        <f>IF(OR(B126="sabun_cuci_tangan",B126="tisu",B126="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4482,7 +4482,7 @@
         <v>15</v>
       </c>
       <c r="F127" t="str">
-        <f>IF(OR(B127="sabun_cuci_tangan",B127="tisu",B127="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
         <v>15</v>
       </c>
       <c r="F128" t="str">
-        <f>IF(OR(B128="sabun_cuci_tangan",B128="tisu",B128="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4528,7 +4528,7 @@
         <v>15</v>
       </c>
       <c r="F129" t="str">
-        <f>IF(OR(B129="sabun_cuci_tangan",B129="tisu",B129="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="3"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4551,7 +4551,7 @@
         <v>16</v>
       </c>
       <c r="F130" t="str">
-        <f>IF(OR(B130="sabun_cuci_tangan",B130="tisu",B130="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F130:F161" si="4">IF(OR(B130="sabun_cuci_tangan",B130="tisu",B130="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -4574,7 +4574,7 @@
         <v>16</v>
       </c>
       <c r="F131" t="str">
-        <f>IF(OR(B131="sabun_cuci_tangan",B131="tisu",B131="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4597,7 +4597,7 @@
         <v>16</v>
       </c>
       <c r="F132" t="str">
-        <f>IF(OR(B132="sabun_cuci_tangan",B132="tisu",B132="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4620,7 +4620,7 @@
         <v>16</v>
       </c>
       <c r="F133" t="str">
-        <f>IF(OR(B133="sabun_cuci_tangan",B133="tisu",B133="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4643,7 +4643,7 @@
         <v>16</v>
       </c>
       <c r="F134" t="str">
-        <f>IF(OR(B134="sabun_cuci_tangan",B134="tisu",B134="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
         <v>16</v>
       </c>
       <c r="F135" t="str">
-        <f>IF(OR(B135="sabun_cuci_tangan",B135="tisu",B135="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4689,7 +4689,7 @@
         <v>16</v>
       </c>
       <c r="F136" t="str">
-        <f>IF(OR(B136="sabun_cuci_tangan",B136="tisu",B136="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4712,7 +4712,7 @@
         <v>16</v>
       </c>
       <c r="F137" t="str">
-        <f>IF(OR(B137="sabun_cuci_tangan",B137="tisu",B137="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4735,7 +4735,7 @@
         <v>16</v>
       </c>
       <c r="F138" t="str">
-        <f>IF(OR(B138="sabun_cuci_tangan",B138="tisu",B138="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
         <v>16</v>
       </c>
       <c r="F139" t="str">
-        <f>IF(OR(B139="sabun_cuci_tangan",B139="tisu",B139="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4781,7 +4781,7 @@
         <v>17</v>
       </c>
       <c r="F140" t="str">
-        <f>IF(OR(B140="sabun_cuci_tangan",B140="tisu",B140="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4804,7 +4804,7 @@
         <v>17</v>
       </c>
       <c r="F141" t="str">
-        <f>IF(OR(B141="sabun_cuci_tangan",B141="tisu",B141="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4827,7 +4827,7 @@
         <v>17</v>
       </c>
       <c r="F142" t="str">
-        <f>IF(OR(B142="sabun_cuci_tangan",B142="tisu",B142="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4850,7 +4850,7 @@
         <v>17</v>
       </c>
       <c r="F143" t="str">
-        <f>IF(OR(B143="sabun_cuci_tangan",B143="tisu",B143="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4873,7 +4873,7 @@
         <v>17</v>
       </c>
       <c r="F144" t="str">
-        <f>IF(OR(B144="sabun_cuci_tangan",B144="tisu",B144="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4896,7 +4896,7 @@
         <v>17</v>
       </c>
       <c r="F145" t="str">
-        <f>IF(OR(B145="sabun_cuci_tangan",B145="tisu",B145="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4919,7 +4919,7 @@
         <v>17</v>
       </c>
       <c r="F146" t="str">
-        <f>IF(OR(B146="sabun_cuci_tangan",B146="tisu",B146="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4942,7 +4942,7 @@
         <v>17</v>
       </c>
       <c r="F147" t="str">
-        <f>IF(OR(B147="sabun_cuci_tangan",B147="tisu",B147="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4965,7 +4965,7 @@
         <v>17</v>
       </c>
       <c r="F148" t="str">
-        <f>IF(OR(B148="sabun_cuci_tangan",B148="tisu",B148="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -4988,7 +4988,7 @@
         <v>17</v>
       </c>
       <c r="F149" t="str">
-        <f>IF(OR(B149="sabun_cuci_tangan",B149="tisu",B149="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5011,7 +5011,7 @@
         <v>18</v>
       </c>
       <c r="F150" t="str">
-        <f>IF(OR(B150="sabun_cuci_tangan",B150="tisu",B150="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5034,7 +5034,7 @@
         <v>18</v>
       </c>
       <c r="F151" t="str">
-        <f>IF(OR(B151="sabun_cuci_tangan",B151="tisu",B151="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
         <v>18</v>
       </c>
       <c r="F152" t="str">
-        <f>IF(OR(B152="sabun_cuci_tangan",B152="tisu",B152="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5080,7 +5080,7 @@
         <v>18</v>
       </c>
       <c r="F153" t="str">
-        <f>IF(OR(B153="sabun_cuci_tangan",B153="tisu",B153="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5103,7 +5103,7 @@
         <v>18</v>
       </c>
       <c r="F154" t="str">
-        <f>IF(OR(B154="sabun_cuci_tangan",B154="tisu",B154="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
         <v>18</v>
       </c>
       <c r="F155" t="str">
-        <f>IF(OR(B155="sabun_cuci_tangan",B155="tisu",B155="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5149,7 +5149,7 @@
         <v>18</v>
       </c>
       <c r="F156" t="str">
-        <f>IF(OR(B156="sabun_cuci_tangan",B156="tisu",B156="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5172,7 +5172,7 @@
         <v>18</v>
       </c>
       <c r="F157" t="str">
-        <f>IF(OR(B157="sabun_cuci_tangan",B157="tisu",B157="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5195,7 +5195,7 @@
         <v>19</v>
       </c>
       <c r="F158" t="str">
-        <f>IF(OR(B158="sabun_cuci_tangan",B158="tisu",B158="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5218,7 +5218,7 @@
         <v>19</v>
       </c>
       <c r="F159" t="str">
-        <f>IF(OR(B159="sabun_cuci_tangan",B159="tisu",B159="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
         <v>19</v>
       </c>
       <c r="F160" t="str">
-        <f>IF(OR(B160="sabun_cuci_tangan",B160="tisu",B160="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
         <v>19</v>
       </c>
       <c r="F161" t="str">
-        <f>IF(OR(B161="sabun_cuci_tangan",B161="tisu",B161="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="4"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
         <v>19</v>
       </c>
       <c r="F162" t="str">
-        <f>IF(OR(B162="sabun_cuci_tangan",B162="tisu",B162="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" ref="F162:F183" si="5">IF(OR(B162="sabun_cuci_tangan",B162="tisu",B162="pengharum_ruangan"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -5310,7 +5310,7 @@
         <v>19</v>
       </c>
       <c r="F163" t="str">
-        <f>IF(OR(B163="sabun_cuci_tangan",B163="tisu",B163="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5333,7 +5333,7 @@
         <v>19</v>
       </c>
       <c r="F164" t="str">
-        <f>IF(OR(B164="sabun_cuci_tangan",B164="tisu",B164="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5356,7 +5356,7 @@
         <v>19</v>
       </c>
       <c r="F165" t="str">
-        <f>IF(OR(B165="sabun_cuci_tangan",B165="tisu",B165="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5379,7 +5379,7 @@
         <v>19</v>
       </c>
       <c r="F166" t="str">
-        <f>IF(OR(B166="sabun_cuci_tangan",B166="tisu",B166="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5402,7 +5402,7 @@
         <v>19</v>
       </c>
       <c r="F167" t="str">
-        <f>IF(OR(B167="sabun_cuci_tangan",B167="tisu",B167="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5425,7 +5425,7 @@
         <v>20</v>
       </c>
       <c r="F168" t="str">
-        <f>IF(OR(B168="sabun_cuci_tangan",B168="tisu",B168="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5448,7 +5448,7 @@
         <v>20</v>
       </c>
       <c r="F169" t="str">
-        <f>IF(OR(B169="sabun_cuci_tangan",B169="tisu",B169="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5471,7 +5471,7 @@
         <v>20</v>
       </c>
       <c r="F170" t="str">
-        <f>IF(OR(B170="sabun_cuci_tangan",B170="tisu",B170="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5494,7 +5494,7 @@
         <v>20</v>
       </c>
       <c r="F171" t="str">
-        <f>IF(OR(B171="sabun_cuci_tangan",B171="tisu",B171="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
         <v>20</v>
       </c>
       <c r="F172" t="str">
-        <f>IF(OR(B172="sabun_cuci_tangan",B172="tisu",B172="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5540,7 +5540,7 @@
         <v>20</v>
       </c>
       <c r="F173" t="str">
-        <f>IF(OR(B173="sabun_cuci_tangan",B173="tisu",B173="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5563,7 +5563,7 @@
         <v>20</v>
       </c>
       <c r="F174" t="str">
-        <f>IF(OR(B174="sabun_cuci_tangan",B174="tisu",B174="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5586,7 +5586,7 @@
         <v>20</v>
       </c>
       <c r="F175" t="str">
-        <f>IF(OR(B175="sabun_cuci_tangan",B175="tisu",B175="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5609,7 +5609,7 @@
         <v>21</v>
       </c>
       <c r="F176" t="str">
-        <f>IF(OR(B176="sabun_cuci_tangan",B176="tisu",B176="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5632,7 +5632,7 @@
         <v>21</v>
       </c>
       <c r="F177" t="str">
-        <f>IF(OR(B177="sabun_cuci_tangan",B177="tisu",B177="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5655,7 +5655,7 @@
         <v>21</v>
       </c>
       <c r="F178" t="str">
-        <f>IF(OR(B178="sabun_cuci_tangan",B178="tisu",B178="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5678,7 +5678,7 @@
         <v>21</v>
       </c>
       <c r="F179" t="str">
-        <f>IF(OR(B179="sabun_cuci_tangan",B179="tisu",B179="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5701,7 +5701,7 @@
         <v>21</v>
       </c>
       <c r="F180" t="str">
-        <f>IF(OR(B180="sabun_cuci_tangan",B180="tisu",B180="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5724,7 +5724,7 @@
         <v>21</v>
       </c>
       <c r="F181" t="str">
-        <f>IF(OR(B181="sabun_cuci_tangan",B181="tisu",B181="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
         <v>21</v>
       </c>
       <c r="F182" t="str">
-        <f>IF(OR(B182="sabun_cuci_tangan",B182="tisu",B182="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -5770,7 +5770,7 @@
         <v>21</v>
       </c>
       <c r="F183" t="str">
-        <f>IF(OR(B183="sabun_cuci_tangan",B183="tisu",B183="pengharum_ruangan"),"refill","non_refill")</f>
+        <f t="shared" si="5"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8715,7 +8715,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -8766,7 +8766,7 @@
         <v>41</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(OR(B2="sabun_cuci_tangan",B2="tisu",B2="pengharum_ruangan",B2="kamper"),"refill","non_refill")</f>
+        <f t="shared" ref="F2:F33" si="0">IF(OR(B2="sabun_cuci_tangan",B2="tisu",B2="pengharum_ruangan",B2="kamper"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -8787,7 +8787,7 @@
         <v>41</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(OR(B3="sabun_cuci_tangan",B3="tisu",B3="pengharum_ruangan",B3="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8808,7 +8808,7 @@
         <v>41</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(OR(B4="sabun_cuci_tangan",B4="tisu",B4="pengharum_ruangan",B4="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
         <v>41</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(OR(B5="sabun_cuci_tangan",B5="tisu",B5="pengharum_ruangan",B5="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8850,7 +8850,7 @@
         <v>41</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(OR(B6="sabun_cuci_tangan",B6="tisu",B6="pengharum_ruangan",B6="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8871,7 +8871,7 @@
         <v>41</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(OR(B7="sabun_cuci_tangan",B7="tisu",B7="pengharum_ruangan",B7="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8892,7 +8892,7 @@
         <v>41</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(OR(B8="sabun_cuci_tangan",B8="tisu",B8="pengharum_ruangan",B8="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8913,7 +8913,7 @@
         <v>41</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(OR(B9="sabun_cuci_tangan",B9="tisu",B9="pengharum_ruangan",B9="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>refill</v>
       </c>
     </row>
@@ -8934,7 +8934,7 @@
         <v>41</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(OR(B10="sabun_cuci_tangan",B10="tisu",B10="pengharum_ruangan",B10="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8955,7 +8955,7 @@
         <v>41</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(OR(B11="sabun_cuci_tangan",B11="tisu",B11="pengharum_ruangan",B11="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8976,7 +8976,7 @@
         <v>41</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(OR(B12="sabun_cuci_tangan",B12="tisu",B12="pengharum_ruangan",B12="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
         <v>42</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(OR(B13="sabun_cuci_tangan",B13="tisu",B13="pengharum_ruangan",B13="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9018,7 +9018,7 @@
         <v>42</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(OR(B14="sabun_cuci_tangan",B14="tisu",B14="pengharum_ruangan",B14="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9039,7 +9039,7 @@
         <v>42</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(OR(B15="sabun_cuci_tangan",B15="tisu",B15="pengharum_ruangan",B15="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9060,7 +9060,7 @@
         <v>42</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(OR(B16="sabun_cuci_tangan",B16="tisu",B16="pengharum_ruangan",B16="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9081,7 +9081,7 @@
         <v>42</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(OR(B17="sabun_cuci_tangan",B17="tisu",B17="pengharum_ruangan",B17="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9102,7 +9102,7 @@
         <v>42</v>
       </c>
       <c r="F18" t="str">
-        <f>IF(OR(B18="sabun_cuci_tangan",B18="tisu",B18="pengharum_ruangan",B18="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9123,7 +9123,7 @@
         <v>42</v>
       </c>
       <c r="F19" t="str">
-        <f>IF(OR(B19="sabun_cuci_tangan",B19="tisu",B19="pengharum_ruangan",B19="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9144,7 +9144,7 @@
         <v>42</v>
       </c>
       <c r="F20" t="str">
-        <f>IF(OR(B20="sabun_cuci_tangan",B20="tisu",B20="pengharum_ruangan",B20="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9165,7 +9165,7 @@
         <v>43</v>
       </c>
       <c r="F21" t="str">
-        <f>IF(OR(B21="sabun_cuci_tangan",B21="tisu",B21="pengharum_ruangan",B21="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9186,7 +9186,7 @@
         <v>43</v>
       </c>
       <c r="F22" t="str">
-        <f>IF(OR(B22="sabun_cuci_tangan",B22="tisu",B22="pengharum_ruangan",B22="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9207,7 +9207,7 @@
         <v>43</v>
       </c>
       <c r="F23" t="str">
-        <f>IF(OR(B23="sabun_cuci_tangan",B23="tisu",B23="pengharum_ruangan",B23="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9228,7 +9228,7 @@
         <v>43</v>
       </c>
       <c r="F24" t="str">
-        <f>IF(OR(B24="sabun_cuci_tangan",B24="tisu",B24="pengharum_ruangan",B24="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9249,7 +9249,7 @@
         <v>43</v>
       </c>
       <c r="F25" t="str">
-        <f>IF(OR(B25="sabun_cuci_tangan",B25="tisu",B25="pengharum_ruangan",B25="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9270,7 +9270,7 @@
         <v>43</v>
       </c>
       <c r="F26" t="str">
-        <f>IF(OR(B26="sabun_cuci_tangan",B26="tisu",B26="pengharum_ruangan",B26="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9291,7 +9291,7 @@
         <v>44</v>
       </c>
       <c r="F27" t="str">
-        <f>IF(OR(B27="sabun_cuci_tangan",B27="tisu",B27="pengharum_ruangan",B27="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9312,7 +9312,7 @@
         <v>44</v>
       </c>
       <c r="F28" t="str">
-        <f>IF(OR(B28="sabun_cuci_tangan",B28="tisu",B28="pengharum_ruangan",B28="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9333,7 +9333,7 @@
         <v>44</v>
       </c>
       <c r="F29" t="str">
-        <f>IF(OR(B29="sabun_cuci_tangan",B29="tisu",B29="pengharum_ruangan",B29="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9354,7 +9354,7 @@
         <v>44</v>
       </c>
       <c r="F30" t="str">
-        <f>IF(OR(B30="sabun_cuci_tangan",B30="tisu",B30="pengharum_ruangan",B30="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9375,7 +9375,7 @@
         <v>44</v>
       </c>
       <c r="F31" t="str">
-        <f>IF(OR(B31="sabun_cuci_tangan",B31="tisu",B31="pengharum_ruangan",B31="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9396,7 +9396,7 @@
         <v>44</v>
       </c>
       <c r="F32" t="str">
-        <f>IF(OR(B32="sabun_cuci_tangan",B32="tisu",B32="pengharum_ruangan",B32="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9417,7 +9417,7 @@
         <v>45</v>
       </c>
       <c r="F33" t="str">
-        <f>IF(OR(B33="sabun_cuci_tangan",B33="tisu",B33="pengharum_ruangan",B33="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="0"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9438,7 +9438,7 @@
         <v>45</v>
       </c>
       <c r="F34" t="str">
-        <f>IF(OR(B34="sabun_cuci_tangan",B34="tisu",B34="pengharum_ruangan",B34="kamper"),"refill","non_refill")</f>
+        <f t="shared" ref="F34:F65" si="1">IF(OR(B34="sabun_cuci_tangan",B34="tisu",B34="pengharum_ruangan",B34="kamper"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -9459,7 +9459,7 @@
         <v>45</v>
       </c>
       <c r="F35" t="str">
-        <f>IF(OR(B35="sabun_cuci_tangan",B35="tisu",B35="pengharum_ruangan",B35="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9480,7 +9480,7 @@
         <v>45</v>
       </c>
       <c r="F36" t="str">
-        <f>IF(OR(B36="sabun_cuci_tangan",B36="tisu",B36="pengharum_ruangan",B36="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9501,7 +9501,7 @@
         <v>45</v>
       </c>
       <c r="F37" t="str">
-        <f>IF(OR(B37="sabun_cuci_tangan",B37="tisu",B37="pengharum_ruangan",B37="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9522,7 +9522,7 @@
         <v>45</v>
       </c>
       <c r="F38" t="str">
-        <f>IF(OR(B38="sabun_cuci_tangan",B38="tisu",B38="pengharum_ruangan",B38="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9543,7 +9543,7 @@
         <v>46</v>
       </c>
       <c r="F39" t="str">
-        <f>IF(OR(B39="sabun_cuci_tangan",B39="tisu",B39="pengharum_ruangan",B39="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9564,7 +9564,7 @@
         <v>46</v>
       </c>
       <c r="F40" t="str">
-        <f>IF(OR(B40="sabun_cuci_tangan",B40="tisu",B40="pengharum_ruangan",B40="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9585,7 +9585,7 @@
         <v>46</v>
       </c>
       <c r="F41" t="str">
-        <f>IF(OR(B41="sabun_cuci_tangan",B41="tisu",B41="pengharum_ruangan",B41="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9606,7 +9606,7 @@
         <v>46</v>
       </c>
       <c r="F42" t="str">
-        <f>IF(OR(B42="sabun_cuci_tangan",B42="tisu",B42="pengharum_ruangan",B42="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9627,7 +9627,7 @@
         <v>46</v>
       </c>
       <c r="F43" t="str">
-        <f>IF(OR(B43="sabun_cuci_tangan",B43="tisu",B43="pengharum_ruangan",B43="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9648,7 +9648,7 @@
         <v>46</v>
       </c>
       <c r="F44" t="str">
-        <f>IF(OR(B44="sabun_cuci_tangan",B44="tisu",B44="pengharum_ruangan",B44="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9669,7 +9669,7 @@
         <v>46</v>
       </c>
       <c r="F45" t="str">
-        <f>IF(OR(B45="sabun_cuci_tangan",B45="tisu",B45="pengharum_ruangan",B45="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9690,7 +9690,7 @@
         <v>47</v>
       </c>
       <c r="F46" t="str">
-        <f>IF(OR(B46="sabun_cuci_tangan",B46="tisu",B46="pengharum_ruangan",B46="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9711,7 +9711,7 @@
         <v>47</v>
       </c>
       <c r="F47" t="str">
-        <f>IF(OR(B47="sabun_cuci_tangan",B47="tisu",B47="pengharum_ruangan",B47="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9732,7 +9732,7 @@
         <v>47</v>
       </c>
       <c r="F48" t="str">
-        <f>IF(OR(B48="sabun_cuci_tangan",B48="tisu",B48="pengharum_ruangan",B48="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9753,7 +9753,7 @@
         <v>47</v>
       </c>
       <c r="F49" t="str">
-        <f>IF(OR(B49="sabun_cuci_tangan",B49="tisu",B49="pengharum_ruangan",B49="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9774,7 +9774,7 @@
         <v>47</v>
       </c>
       <c r="F50" t="str">
-        <f>IF(OR(B50="sabun_cuci_tangan",B50="tisu",B50="pengharum_ruangan",B50="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
         <v>47</v>
       </c>
       <c r="F51" t="str">
-        <f>IF(OR(B51="sabun_cuci_tangan",B51="tisu",B51="pengharum_ruangan",B51="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9816,7 +9816,7 @@
         <v>47</v>
       </c>
       <c r="F52" t="str">
-        <f>IF(OR(B52="sabun_cuci_tangan",B52="tisu",B52="pengharum_ruangan",B52="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9837,7 +9837,7 @@
         <v>48</v>
       </c>
       <c r="F53" t="str">
-        <f>IF(OR(B53="sabun_cuci_tangan",B53="tisu",B53="pengharum_ruangan",B53="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9858,7 +9858,7 @@
         <v>48</v>
       </c>
       <c r="F54" t="str">
-        <f>IF(OR(B54="sabun_cuci_tangan",B54="tisu",B54="pengharum_ruangan",B54="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9879,7 +9879,7 @@
         <v>48</v>
       </c>
       <c r="F55" t="str">
-        <f>IF(OR(B55="sabun_cuci_tangan",B55="tisu",B55="pengharum_ruangan",B55="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9900,7 +9900,7 @@
         <v>48</v>
       </c>
       <c r="F56" t="str">
-        <f>IF(OR(B56="sabun_cuci_tangan",B56="tisu",B56="pengharum_ruangan",B56="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9921,7 +9921,7 @@
         <v>48</v>
       </c>
       <c r="F57" t="str">
-        <f>IF(OR(B57="sabun_cuci_tangan",B57="tisu",B57="pengharum_ruangan",B57="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9942,7 +9942,7 @@
         <v>48</v>
       </c>
       <c r="F58" t="str">
-        <f>IF(OR(B58="sabun_cuci_tangan",B58="tisu",B58="pengharum_ruangan",B58="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9963,7 +9963,7 @@
         <v>49</v>
       </c>
       <c r="F59" t="str">
-        <f>IF(OR(B59="sabun_cuci_tangan",B59="tisu",B59="pengharum_ruangan",B59="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -9984,7 +9984,7 @@
         <v>49</v>
       </c>
       <c r="F60" t="str">
-        <f>IF(OR(B60="sabun_cuci_tangan",B60="tisu",B60="pengharum_ruangan",B60="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10005,7 +10005,7 @@
         <v>49</v>
       </c>
       <c r="F61" t="str">
-        <f>IF(OR(B61="sabun_cuci_tangan",B61="tisu",B61="pengharum_ruangan",B61="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10026,7 +10026,7 @@
         <v>49</v>
       </c>
       <c r="F62" t="str">
-        <f>IF(OR(B62="sabun_cuci_tangan",B62="tisu",B62="pengharum_ruangan",B62="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10047,7 +10047,7 @@
         <v>49</v>
       </c>
       <c r="F63" t="str">
-        <f>IF(OR(B63="sabun_cuci_tangan",B63="tisu",B63="pengharum_ruangan",B63="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10068,7 +10068,7 @@
         <v>49</v>
       </c>
       <c r="F64" t="str">
-        <f>IF(OR(B64="sabun_cuci_tangan",B64="tisu",B64="pengharum_ruangan",B64="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10089,7 +10089,7 @@
         <v>50</v>
       </c>
       <c r="F65" t="str">
-        <f>IF(OR(B65="sabun_cuci_tangan",B65="tisu",B65="pengharum_ruangan",B65="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="1"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10110,7 +10110,7 @@
         <v>50</v>
       </c>
       <c r="F66" t="str">
-        <f>IF(OR(B66="sabun_cuci_tangan",B66="tisu",B66="pengharum_ruangan",B66="kamper"),"refill","non_refill")</f>
+        <f t="shared" ref="F66:F81" si="2">IF(OR(B66="sabun_cuci_tangan",B66="tisu",B66="pengharum_ruangan",B66="kamper"),"refill","non_refill")</f>
         <v>non_refill</v>
       </c>
     </row>
@@ -10131,7 +10131,7 @@
         <v>50</v>
       </c>
       <c r="F67" t="str">
-        <f>IF(OR(B67="sabun_cuci_tangan",B67="tisu",B67="pengharum_ruangan",B67="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10152,7 +10152,7 @@
         <v>50</v>
       </c>
       <c r="F68" t="str">
-        <f>IF(OR(B68="sabun_cuci_tangan",B68="tisu",B68="pengharum_ruangan",B68="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10173,7 +10173,7 @@
         <v>50</v>
       </c>
       <c r="F69" t="str">
-        <f>IF(OR(B69="sabun_cuci_tangan",B69="tisu",B69="pengharum_ruangan",B69="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10194,7 +10194,7 @@
         <v>50</v>
       </c>
       <c r="F70" t="str">
-        <f>IF(OR(B70="sabun_cuci_tangan",B70="tisu",B70="pengharum_ruangan",B70="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10215,7 +10215,7 @@
         <v>50</v>
       </c>
       <c r="F71" t="str">
-        <f>IF(OR(B71="sabun_cuci_tangan",B71="tisu",B71="pengharum_ruangan",B71="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10236,7 +10236,7 @@
         <v>50</v>
       </c>
       <c r="F72" t="str">
-        <f>IF(OR(B72="sabun_cuci_tangan",B72="tisu",B72="pengharum_ruangan",B72="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>refill</v>
       </c>
     </row>
@@ -10257,7 +10257,7 @@
         <v>50</v>
       </c>
       <c r="F73" t="str">
-        <f>IF(OR(B73="sabun_cuci_tangan",B73="tisu",B73="pengharum_ruangan",B73="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10278,7 +10278,7 @@
         <v>50</v>
       </c>
       <c r="F74" t="str">
-        <f>IF(OR(B74="sabun_cuci_tangan",B74="tisu",B74="pengharum_ruangan",B74="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10299,7 +10299,7 @@
         <v>50</v>
       </c>
       <c r="F75" t="str">
-        <f>IF(OR(B75="sabun_cuci_tangan",B75="tisu",B75="pengharum_ruangan",B75="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10320,7 +10320,7 @@
         <v>51</v>
       </c>
       <c r="F76" t="str">
-        <f>IF(OR(B76="sabun_cuci_tangan",B76="tisu",B76="pengharum_ruangan",B76="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10341,7 +10341,7 @@
         <v>51</v>
       </c>
       <c r="F77" t="str">
-        <f>IF(OR(B77="sabun_cuci_tangan",B77="tisu",B77="pengharum_ruangan",B77="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10362,7 +10362,7 @@
         <v>51</v>
       </c>
       <c r="F78" t="str">
-        <f>IF(OR(B78="sabun_cuci_tangan",B78="tisu",B78="pengharum_ruangan",B78="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10383,7 +10383,7 @@
         <v>51</v>
       </c>
       <c r="F79" t="str">
-        <f>IF(OR(B79="sabun_cuci_tangan",B79="tisu",B79="pengharum_ruangan",B79="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10404,7 +10404,7 @@
         <v>51</v>
       </c>
       <c r="F80" t="str">
-        <f>IF(OR(B80="sabun_cuci_tangan",B80="tisu",B80="pengharum_ruangan",B80="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
@@ -10425,7 +10425,7 @@
         <v>51</v>
       </c>
       <c r="F81" t="str">
-        <f>IF(OR(B81="sabun_cuci_tangan",B81="tisu",B81="pengharum_ruangan",B81="kamper"),"refill","non_refill")</f>
+        <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor(checklist_kebersihan): Memperbaiki excel untuk data checklist kebersihan
</commit_message>
<xml_diff>
--- a/cheklist_kebersihan.xlsx
+++ b/cheklist_kebersihan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp2\Documents\Bionic\bionic\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D029ACE-1D93-446D-8900-275A311F5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE579B7-B8CA-4270-8091-F5776F893026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="1245" windowWidth="21015" windowHeight="11295" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="1245" windowWidth="21015" windowHeight="11295" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shift 1" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="312">
   <si>
     <t>bersih</t>
   </si>
@@ -978,6 +978,9 @@
   </si>
   <si>
     <t>id_item_type</t>
+  </si>
+  <si>
+    <t>Laundry APD</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1228,6 +1231,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1554,7 +1560,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A96" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -5800,10 +5806,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8507,20 +8513,20 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="11" t="s">
-        <v>10</v>
+      <c r="A129" s="8" t="s">
+        <v>311</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>308</v>
+        <v>199</v>
       </c>
       <c r="C129" s="8"/>
       <c r="D129" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B129,all_items!$A$1:$A$57,0))), "")</f>
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="E129" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A129,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F129" s="5" t="str">
         <f t="shared" si="1"/>
@@ -8528,20 +8534,20 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="11" t="s">
-        <v>10</v>
+      <c r="A130" s="8" t="s">
+        <v>311</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C130" s="8"/>
+        <v>200</v>
+      </c>
+      <c r="C130" s="28"/>
       <c r="D130" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B130,all_items!$A$1:$A$57,0))), "")</f>
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E130" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A130,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F130" s="5" t="str">
         <f t="shared" si="1"/>
@@ -8550,19 +8556,19 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C131" s="8"/>
+        <v>201</v>
+      </c>
+      <c r="C131" s="28"/>
       <c r="D131" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B131,all_items!$A$1:$A$57,0))), "")</f>
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E131" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A131,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F131" s="5" t="str">
         <f t="shared" ref="F131:F135" si="2">IF(OR(B131="sabun_cuci_tangan",B131="tisu",B131="pengharum_ruangan",B131="kamper"),"refill","non_refill")</f>
@@ -8571,19 +8577,19 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C132" s="8"/>
+        <v>202</v>
+      </c>
+      <c r="C132" s="28"/>
       <c r="D132" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B132,all_items!$A$1:$A$57,0))), "")</f>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E132" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A132,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F132" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8592,19 +8598,19 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C133" s="8"/>
+        <v>203</v>
+      </c>
+      <c r="C133" s="28"/>
       <c r="D133" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B133,all_items!$A$1:$A$57,0))), "")</f>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E133" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A133,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F133" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8613,19 +8619,19 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C134" s="8"/>
+        <v>204</v>
+      </c>
+      <c r="C134" s="28"/>
       <c r="D134" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B134,all_items!$A$1:$A$57,0))), "")</f>
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E134" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A134,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F134" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8634,73 +8640,150 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C135" s="8"/>
+        <v>205</v>
+      </c>
+      <c r="C135" s="28"/>
       <c r="D135" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B135,all_items!$A$1:$A$57,0))), "")</f>
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E135" s="7">
         <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A135,all_locations!$E$1:$E$51,0))), "")</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F135" s="5" t="str">
         <f t="shared" si="2"/>
         <v>non_refill</v>
       </c>
     </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C136" s="8"/>
+      <c r="D136" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B136,all_items!$A$1:$A$57,0))), "")</f>
+        <v>1</v>
+      </c>
+      <c r="E136" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A136,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F136" s="5" t="str">
+        <f>IF(OR(B136="sabun_cuci_tangan",B136="tisu",B136="pengharum_ruangan",B136="kamper"),"refill","non_refill")</f>
+        <v>non_refill</v>
+      </c>
+    </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
-      <c r="D137"/>
-      <c r="E137"/>
+      <c r="A137" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C137" s="8"/>
+      <c r="D137" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B137,all_items!$A$1:$A$57,0))), "")</f>
+        <v>2</v>
+      </c>
+      <c r="E137" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A137,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F137" s="5" t="str">
+        <f t="shared" ref="F137:F141" si="3">IF(OR(B137="sabun_cuci_tangan",B137="tisu",B137="pengharum_ruangan",B137="kamper"),"refill","non_refill")</f>
+        <v>non_refill</v>
+      </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
-      <c r="D138"/>
-      <c r="E138"/>
+      <c r="A138" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C138" s="8"/>
+      <c r="D138" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B138,all_items!$A$1:$A$57,0))), "")</f>
+        <v>5</v>
+      </c>
+      <c r="E138" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A138,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F138" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>non_refill</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
-      <c r="D139"/>
-      <c r="E139"/>
+      <c r="A139" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C139" s="8"/>
+      <c r="D139" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B139,all_items!$A$1:$A$57,0))), "")</f>
+        <v>49</v>
+      </c>
+      <c r="E139" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A139,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F139" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>non_refill</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
-      <c r="D140"/>
-      <c r="E140"/>
+      <c r="A140" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C140" s="8"/>
+      <c r="D140" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B140,all_items!$A$1:$A$57,0))), "")</f>
+        <v>50</v>
+      </c>
+      <c r="E140" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A140,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F140" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>non_refill</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
-      <c r="D141"/>
-      <c r="E141"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
-      <c r="D142"/>
-      <c r="E142"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
-      <c r="D143"/>
-      <c r="E143"/>
+      <c r="A141" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C141" s="8"/>
+      <c r="D141" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_items!$A$1:$A$57,MATCH(B141,all_items!$A$1:$A$57,0))), "")</f>
+        <v>51</v>
+      </c>
+      <c r="E141" s="7">
+        <f>_xlfn.IFNA(ROW(INDEX(all_locations!$E$1:$E$51,MATCH(A141,all_locations!$E$1:$E$51,0))), "")</f>
+        <v>40</v>
+      </c>
+      <c r="F141" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>non_refill</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E135">
@@ -8715,7 +8798,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -10448,8 +10531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10906,10 +10989,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B131"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:XFD116"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11848,169 +11931,121 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>206</v>
       </c>
       <c r="B117" t="s">
-        <v>199</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>308</v>
+        <v>206</v>
       </c>
       <c r="B118" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>206</v>
       </c>
       <c r="B119" t="s">
-        <v>201</v>
+        <v>285</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>308</v>
+        <v>207</v>
       </c>
       <c r="B120" t="s">
-        <v>202</v>
+        <v>282</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>308</v>
+        <v>207</v>
       </c>
       <c r="B121" t="s">
-        <v>203</v>
+        <v>281</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>308</v>
+        <v>208</v>
       </c>
       <c r="B122" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B123" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B124" t="s">
-        <v>284</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B125" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B126" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B127" t="s">
-        <v>281</v>
+        <v>155</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B128" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B129" t="s">
-        <v>283</v>
+        <v>157</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B130" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B131" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>209</v>
-      </c>
-      <c r="B132" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>210</v>
-      </c>
-      <c r="B133" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>210</v>
-      </c>
-      <c r="B134" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>211</v>
-      </c>
-      <c r="B135" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>212</v>
-      </c>
-      <c r="B136" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>212</v>
-      </c>
-      <c r="B137" t="s">
         <v>154</v>
       </c>
     </row>
@@ -12023,7 +12058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D31" workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>